<commit_message>
Update of regular expressions for identifying tracking cookies
</commit_message>
<xml_diff>
--- a/lessonslearned_1pm.xlsx
+++ b/lessonslearned_1pm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="645" windowWidth="18555" windowHeight="7425"/>
+    <workbookView xWindow="600" yWindow="645" windowWidth="15480" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>mac address for gateway - id for wifi</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>ask ghostery if we can use their database</t>
+  </si>
+  <si>
+    <t>00:00:0c:07:ac:0e</t>
   </si>
 </sst>
 </file>
@@ -161,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -174,9 +177,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -214,7 +217,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -286,7 +289,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -462,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +504,9 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">

</xml_diff>